<commit_message>
Remove extra "other" option in Q54b
</commit_message>
<xml_diff>
--- a/odkx/forms/census.xlsx
+++ b/odkx/forms/census.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -996,265 +996,265 @@
     <t xml:space="preserve">selected(data('hh_spray'), 'yes')</t>
   </si>
   <si>
+    <t xml:space="preserve">hh_spray_label_seen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54b. Was the spray registry label seen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data('hh_spray_label_seen'), 'yes')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_no_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_spray_label_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54b(i). Spray date (verify date on the fumigation registry label on the door)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_num_nets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55. How many mosquito nets are there in the household?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('hh_num_nets') &lt; 51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannot exceed 50.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data('hh_num_nets') &gt; 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h5&gt;You will be prompted to answer additional questions for each of the {{data.hh_num_nets}} nets.&lt;/h5&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mosquito Net Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_mosquito_net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;Add mosquito net&lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">malaria_prevention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">malaria_prevention_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56. Are any other malaria prevention methods used? (click all that apply)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health and Morbidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;Health / Morbidity Information&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choices_hf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">health_facility_formal_sick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57. What is the first point of formal health care used by the family when someone is sick?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data('health_facility_formal_sick'), 'other')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">health_facility_formal_non_severe_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snake bites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h4&gt;Snake bite&lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yndkpna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">any_snake_bite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58. Has any household member been bitten by a snake in the past 12 months?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data('any_snake_bite'), 'yes')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">any_snake_bite_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58a. How many household members were bitten in the past 12 months?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h5&gt;You will be prompted to answer additional questions for the {{data.any_snake_bite_num}} individual(s) who have experienced a snake bite.&lt;/h5&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snake Bite details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake_bite_who</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59a. Who was bitten?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_member_snake_bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h5&gt;Answer additional questions for the individual(s) who have experienced a snake bite.&lt;/h5&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_.contains(data('snake_bite_who'), choice_item.instance_id)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60. Contact number for household</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_contact_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_contact_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_contact_alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61. Alternative contact number 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_alt_contact_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_contact_alt_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!!data('hh_contact_alt')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_contact_alt_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62. Is there an alternative contact number 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_contact_alt_2_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62a. Alternative contact number 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_for_project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63. Can we call you on any one of the contact numbers indicated above to arrange visits with you in the context of this project?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;Deaths in the past 12 months&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For new households only (households that were not part of minicensus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64. Have there been any deaths in the household in the past 12 months?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data('hh_death'), 'yes')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hh_death_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64a. How many?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h5&gt;You will be prompted to answer additional questions for each of the {{data.hh_death_count }} death(s).&lt;/h5&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_hh_death</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual Form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;INDIVIDUAL QUESTIONNAIRE&lt;/h2&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are about to begin the individual questionnaire. For each RESIDENT member in the household, a separate form will be filled out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">member_questionnaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">display.title.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ynpna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefer not to answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't Know</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ynna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Applicable</t>
+  </si>
+  <si>
     <t xml:space="preserve">yno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_spray_label_seen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54b. Was the spray registry label seen?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(data('hh_spray_label_seen'), 'yes')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_no_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_spray_label_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54b(i). Spray date (verify date on the fumigation registry label on the door)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_num_nets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55. How many mosquito nets are there in the household?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data('hh_num_nets') &lt; 51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cannot exceed 50.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data('hh_num_nets') &gt; 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h5&gt;You will be prompted to answer additional questions for each of the {{data.hh_num_nets}} nets.&lt;/h5&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mosquito Net Details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linked_mosquito_net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h4&gt;Add mosquito net&lt;/h4&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">malaria_prevention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">malaria_prevention_method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56. Are any other malaria prevention methods used? (click all that apply)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Health and Morbidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h2&gt;Health / Morbidity Information&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choices_hf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_facility_formal_sick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57. What is the first point of formal health care used by the family when someone is sick?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(data('health_facility_formal_sick'), 'other')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">health_facility_formal_non_severe_other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snake bites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h4&gt;Snake bite&lt;/h4&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yndkpna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">any_snake_bite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58. Has any household member been bitten by a snake in the past 12 months?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(data('any_snake_bite'), 'yes')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">any_snake_bite_num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58a. How many household members were bitten in the past 12 months?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h5&gt;You will be prompted to answer additional questions for the {{data.any_snake_bite_num}} individual(s) who have experienced a snake bite.&lt;/h5&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snake Bite details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">snake_bite_who</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59a. Who was bitten?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linked_member_snake_bit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h5&gt;Answer additional questions for the individual(s) who have experienced a snake bite.&lt;/h5&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_.contains(data('snake_bite_who'), choice_item.instance_id)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60. Contact number for household</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_contact_num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_contact_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_contact_alt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61. Alternative contact number 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no_alt_contact_num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_contact_alt_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!!data('hh_contact_alt')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_contact_alt_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62. Is there an alternative contact number 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_contact_alt_2_num</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62a. Alternative contact number 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact_for_project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63. Can we call you on any one of the contact numbers indicated above to arrange visits with you in the context of this project?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h2&gt;Deaths in the past 12 months&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For new households only (households that were not part of minicensus)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64. Have there been any deaths in the household in the past 12 months?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selected(data('hh_death'), 'yes')</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hh_death_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64a. How many?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h5&gt;You will be prompted to answer additional questions for each of the {{data.hh_death_count }} death(s).&lt;/h5&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linked_hh_death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual Form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h2&gt;INDIVIDUAL QUESTIONNAIRE&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You are about to begin the individual questionnaire. For each RESIDENT member in the household, a separate form will be filled out. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">member_questionnaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">display.title.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ynpna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prefer not to answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Don't Know</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ynna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Applicable</t>
   </si>
   <si>
     <t xml:space="preserve">other</t>
@@ -6866,7 +6866,7 @@
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.46875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7108,7 +7108,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.49"/>
@@ -7172,7 +7172,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -7187,10 +7187,10 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -7202,11 +7202,11 @@
         <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -7247,12 +7247,12 @@
   <dimension ref="A1:C1724"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A1706" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A222" activeCellId="0" sqref="A222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="66.32"/>
@@ -7260,13 +7260,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7274,10 +7274,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7285,43 +7285,43 @@
         <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7329,10 +7329,10 @@
         <v>162</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7340,10 +7340,10 @@
         <v>162</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7351,114 +7351,114 @@
         <v>162</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>320</v>
+        <v>406</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>320</v>
+        <v>406</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>320</v>
+        <v>406</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>407</v>
@@ -7549,10 +7549,10 @@
         <v>416</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7593,10 +7593,10 @@
         <v>419</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7733,13 +7733,13 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7780,10 +7780,10 @@
         <v>451</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7813,10 +7813,10 @@
         <v>451</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7967,7 +7967,7 @@
         <v>458</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>485</v>
@@ -8022,10 +8022,10 @@
         <v>487</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8077,7 +8077,7 @@
         <v>490</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>485</v>
@@ -8198,7 +8198,7 @@
         <v>497</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>485</v>
@@ -8209,10 +8209,10 @@
         <v>497</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8418,7 +8418,7 @@
         <v>524</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>485</v>
@@ -8517,7 +8517,7 @@
         <v>530</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>485</v>
@@ -8671,10 +8671,10 @@
         <v>259</v>
       </c>
       <c r="B129" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9595,10 +9595,10 @@
         <v>159</v>
       </c>
       <c r="B213" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C213" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10299,10 +10299,10 @@
         <v>244</v>
       </c>
       <c r="B277" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C277" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C277" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10420,7 +10420,7 @@
         <v>244</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>688</v>
@@ -10530,10 +10530,10 @@
         <v>237</v>
       </c>
       <c r="B298" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C298" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10541,7 +10541,7 @@
         <v>237</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>688</v>
@@ -10585,10 +10585,10 @@
         <v>286</v>
       </c>
       <c r="B303" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C303" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C303" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10706,7 +10706,7 @@
         <v>286</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C314" s="1" t="s">
         <v>688</v>
@@ -10761,7 +10761,7 @@
         <v>316</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>688</v>
@@ -10783,10 +10783,10 @@
         <v>316</v>
       </c>
       <c r="B321" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C321" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C321" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10838,7 +10838,7 @@
         <v>818</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C326" s="1" t="s">
         <v>485</v>
@@ -10948,7 +10948,7 @@
         <v>825</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C336" s="1" t="s">
         <v>485</v>
@@ -10959,7 +10959,7 @@
         <v>842</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C337" s="1" t="s">
         <v>843</v>
@@ -11157,10 +11157,10 @@
         <v>866</v>
       </c>
       <c r="B355" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C355" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C355" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12389,7 +12389,7 @@
         <v>878</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C467" s="1" t="s">
         <v>688</v>
@@ -12400,10 +12400,10 @@
         <v>878</v>
       </c>
       <c r="B468" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C468" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C468" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13533,7 +13533,7 @@
         <v>971</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C571" s="1" t="s">
         <v>485</v>
@@ -13544,7 +13544,7 @@
         <v>971</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C572" s="1" t="s">
         <v>996</v>
@@ -13566,10 +13566,10 @@
         <v>971</v>
       </c>
       <c r="B574" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C574" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C574" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13720,10 +13720,10 @@
         <v>997</v>
       </c>
       <c r="B588" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C588" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C588" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14270,7 +14270,7 @@
         <v>1065</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C638" s="1" t="s">
         <v>1069</v>
@@ -14325,7 +14325,7 @@
         <v>1070</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C643" s="1" t="s">
         <v>485</v>
@@ -14413,10 +14413,10 @@
         <v>1075</v>
       </c>
       <c r="B651" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C651" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C651" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14457,10 +14457,10 @@
         <v>1084</v>
       </c>
       <c r="B655" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C655" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="C655" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14468,10 +14468,10 @@
         <v>1084</v>
       </c>
       <c r="B656" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C656" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C656" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14501,7 +14501,7 @@
         <v>1089</v>
       </c>
       <c r="B659" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C659" s="1" t="s">
         <v>688</v>
@@ -14523,10 +14523,10 @@
         <v>1089</v>
       </c>
       <c r="B661" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C661" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="C661" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14556,10 +14556,10 @@
         <v>1096</v>
       </c>
       <c r="B664" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14644,10 +14644,10 @@
         <v>1105</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14655,10 +14655,10 @@
         <v>1105</v>
       </c>
       <c r="B673" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C673" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C673" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14710,10 +14710,10 @@
         <v>1110</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C678" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14864,10 +14864,10 @@
         <v>1129</v>
       </c>
       <c r="B692" s="37" t="s">
+        <v>402</v>
+      </c>
+      <c r="C692" s="37" t="s">
         <v>403</v>
-      </c>
-      <c r="C692" s="37" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15950,10 +15950,10 @@
     </row>
     <row r="791" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A791" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C791" s="1" t="s">
         <v>1212</v>
@@ -15961,10 +15961,10 @@
     </row>
     <row r="792" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A792" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B792" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C792" s="1" t="s">
         <v>1213</v>
@@ -16030,10 +16030,10 @@
         <v>1214</v>
       </c>
       <c r="B798" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C798" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C798" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="799" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24907,10 +24907,10 @@
         <v>2000</v>
       </c>
       <c r="B1605" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1605" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C1605" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="1606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25050,10 +25050,10 @@
         <v>2001</v>
       </c>
       <c r="B1618" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C1618" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C1618" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="1619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26172,7 +26172,7 @@
         <v>2015</v>
       </c>
       <c r="B1720" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C1720" s="1" t="s">
         <v>688</v>
@@ -26244,7 +26244,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.07"/>
@@ -26296,7 +26296,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.94"/>
@@ -26395,7 +26395,7 @@
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.37"/>
@@ -26410,7 +26410,7 @@
         <v>2031</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26563,7 +26563,7 @@
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.72"/>
@@ -26571,7 +26571,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="65.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.31"/>
@@ -26611,7 +26611,7 @@
     </row>
     <row r="2" customFormat="false" ht="48.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2074</v>
@@ -26711,7 +26711,7 @@
     </row>
     <row r="7" customFormat="false" ht="48.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2074</v>
@@ -26731,7 +26731,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>38</v>
@@ -26739,10 +26739,10 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>2085</v>
@@ -26983,7 +26983,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>38</v>
@@ -27039,7 +27039,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>38</v>
@@ -27067,7 +27067,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>38</v>
@@ -27143,7 +27143,22 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="13" style="0" width="10.75"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
@@ -27415,7 +27430,7 @@
       <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.73"/>
@@ -28170,12 +28185,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="77.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.68"/>
@@ -28301,11 +28316,11 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.04"/>
@@ -28565,7 +28580,7 @@
       <selection pane="bottomLeft" activeCell="D62" activeCellId="0" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.63"/>
@@ -29576,7 +29591,7 @@
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="35.42"/>
@@ -31715,23 +31730,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1048576"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="50.37"/>
@@ -32170,13 +32183,13 @@
         <v>113</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -32191,7 +32204,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -32209,14 +32222,14 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -32285,17 +32298,17 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>330</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -32307,7 +32320,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -32330,7 +32343,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -32364,7 +32377,7 @@
       <c r="D32" s="32"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
@@ -32381,11 +32394,11 @@
         <v>38</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -32453,13 +32466,13 @@
         <v>60</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -32514,7 +32527,7 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -32533,7 +32546,7 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -32550,13 +32563,13 @@
         <v>87</v>
       </c>
       <c r="D42" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="E42" s="32" t="s">
         <v>341</v>
       </c>
-      <c r="E42" s="32" t="s">
+      <c r="F42" s="32" t="s">
         <v>342</v>
-      </c>
-      <c r="F42" s="32" t="s">
-        <v>343</v>
       </c>
       <c r="G42" s="32"/>
       <c r="H42" s="32"/>
@@ -32573,7 +32586,7 @@
         <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -32595,7 +32608,7 @@
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>127</v>
@@ -32668,7 +32681,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -32687,7 +32700,7 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -32704,13 +32717,13 @@
         <v>31</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -32725,7 +32738,7 @@
         <v>14</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -32747,10 +32760,10 @@
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>353</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -32769,7 +32782,7 @@
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -32788,7 +32801,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -32808,10 +32821,10 @@
         <v>54</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -32828,17 +32841,17 @@
         <v>38</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K56" s="1"/>
       <c r="L56" s="1" t="n">
@@ -32907,7 +32920,7 @@
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -32925,10 +32938,10 @@
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -32937,7 +32950,7 @@
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32947,13 +32960,13 @@
         <v>60</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>367</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -32971,10 +32984,10 @@
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -32983,7 +32996,7 @@
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32993,13 +33006,13 @@
         <v>60</v>
       </c>
       <c r="D64" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>371</v>
-      </c>
       <c r="F64" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -33014,7 +33027,7 @@
         <v>14</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C65" s="32"/>
       <c r="D65" s="32"/>
@@ -33038,10 +33051,10 @@
         <v>44</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>373</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>374</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -33059,10 +33072,10 @@
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>375</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -33071,7 +33084,7 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33101,10 +33114,10 @@
         <v>162</v>
       </c>
       <c r="E69" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>377</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>378</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -33131,9 +33144,6 @@
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -33156,7 +33166,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -33212,7 +33222,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33220,7 +33230,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33231,10 +33241,10 @@
         <v>44</v>
       </c>
       <c r="E5" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>381</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33242,7 +33252,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33250,10 +33260,10 @@
         <v>50</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>384</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>385</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>1</v>
@@ -33267,7 +33277,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33275,7 +33285,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update member roster wording
</commit_message>
<xml_diff>
--- a/odkx/forms/census.xlsx
+++ b/odkx/forms/census.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">Current Household Members Roster</t>
   </si>
   <si>
-    <t xml:space="preserve">data('roster_counter') === 0</t>
+    <t xml:space="preserve">data('roster_count') === 0</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;i&gt;Empty&lt;/i&gt;</t>
@@ -256,7 +256,7 @@
     <t xml:space="preserve">hh_minicenced_members_correct</t>
   </si>
   <si>
-    <t xml:space="preserve">Is this list correct?</t>
+    <t xml:space="preserve">Have any members left the household?</t>
   </si>
   <si>
     <t xml:space="preserve">selected(data('hh_minicenced_members_correct'), 'no')</t>
@@ -7011,7 +7011,7 @@
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -7253,7 +7253,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.49"/>
@@ -7435,7 +7435,7 @@
       <selection pane="bottomLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="66.32"/>
@@ -26457,7 +26457,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.07"/>
@@ -26509,12 +26509,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.3"/>
   </cols>
   <sheetData>
@@ -26604,11 +26604,11 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.6"/>
@@ -26882,7 +26882,7 @@
       <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.72"/>
@@ -27462,7 +27462,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.27"/>
@@ -27506,7 +27506,7 @@
       <selection pane="topLeft" activeCell="P9" activeCellId="0" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.49"/>
@@ -27832,13 +27832,13 @@
   </sheetPr>
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.73"/>
@@ -28932,7 +28932,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.49"/>
@@ -29065,7 +29065,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.04"/>
@@ -29360,7 +29360,7 @@
       <selection pane="bottomLeft" activeCell="L60" activeCellId="0" sqref="L60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.63"/>
@@ -30785,7 +30785,7 @@
       <selection pane="bottomLeft" activeCell="D112" activeCellId="0" sqref="D112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="35.42"/>
@@ -33471,7 +33471,7 @@
       <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.63"/>
@@ -35454,7 +35454,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.33984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.13"/>

</xml_diff>

<commit_message>
Fix linked instance counting
</commit_message>
<xml_diff>
--- a/odkx/forms/census.xlsx
+++ b/odkx/forms/census.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5779" uniqueCount="2156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5771" uniqueCount="2174">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -6395,6 +6395,9 @@
   </si>
   <si>
     <t xml:space="preserve">comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subFormStatusCol</t>
   </si>
   <si>
     <t xml:space="preserve">csv</t>
@@ -6463,7 +6466,13 @@
     <t xml:space="preserve">hh_member</t>
   </si>
   <si>
-    <t xml:space="preserve">linked_hh_member</t>
+    <t xml:space="preserve">{ hh_id: data('hh_id'), form_status_hh_member: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ form_status_hh_member: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_status_hh_member</t>
   </si>
   <si>
     <t xml:space="preserve">hh_member_absent</t>
@@ -6475,28 +6484,73 @@
     <t xml:space="preserve">[ data('hh_id'), 'resident' ]</t>
   </si>
   <si>
+    <t xml:space="preserve">{ hh_id: data('hh_id'), form_status_hh_member_absent: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ form_status_hh_member_absent: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_status_hh_member_absent</t>
+  </si>
+  <si>
     <t xml:space="preserve">hh_member_exit</t>
   </si>
   <si>
+    <t xml:space="preserve">{ hh_id: data('hh_id'), form_status_hh_member_exit: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ form_status_hh_member_exit: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_status_hh_member_exit</t>
+  </si>
+  <si>
     <t xml:space="preserve">hh_member_new</t>
   </si>
   <si>
-    <t xml:space="preserve">{ hh_id: data('hh_id'), hh_country: data('hh_country'), id_candidate: data('id_candidate') }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ id_candidate: data('id_candidate') }</t>
+    <t xml:space="preserve">{ hh_id: data('hh_id'), hh_country: data('hh_country'), id_candidate: data('id_candidate'), form_status_hh_member_new: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ id_candidate: data('id_candidate'), form_status_hh_member_new: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_status_hh_member_new</t>
   </si>
   <si>
     <t xml:space="preserve">hh_member_questions</t>
   </si>
   <si>
-    <t xml:space="preserve">{ hh_head: data('hh_head_new_select') }</t>
+    <t xml:space="preserve">{ hh_id: data('hh_id'), form_status_hh_member_questions: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ hh_head: data('hh_head_new_select'), form_status_hh_member_questions: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_status_hh_member_questions</t>
   </si>
   <si>
     <t xml:space="preserve">hh_new_member_new</t>
   </si>
   <si>
+    <t xml:space="preserve">{ hh_id: data('hh_id'), hh_country: data('hh_country'), id_candidate: data('id_candidate'), form_status_hh_new_member_new: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ id_candidate: data('id_candidate'), form_status_hh_new_member_new: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_status_hh_new_member_new</t>
+  </si>
+  <si>
     <t xml:space="preserve">hh_member_snake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ hh_id: data('hh_id'), form_status_hh_member_snake: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ form_status_hh_member_snake: 1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_status_hh_member_snake</t>
   </si>
   <si>
     <t xml:space="preserve">hh_mosquito_net</t>
@@ -25018,7 +25072,7 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -25071,7 +25125,7 @@
         <v>2085</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>20210203001</v>
+        <v>20210205001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25288,15 +25342,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.72"/>
@@ -25308,6 +25362,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="76.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="34.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25344,19 +25399,22 @@
       <c r="K1" s="0" t="s">
         <v>2119</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>2120</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="48.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>379</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2121</v>
+        <v>2122</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>2122</v>
+        <v>2123</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -25370,13 +25428,13 @@
         <v>150</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2123</v>
+        <v>2124</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>2124</v>
+        <v>2125</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -25390,13 +25448,13 @@
         <v>161</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>2126</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>2125</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>2124</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -25410,13 +25468,13 @@
         <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2126</v>
+        <v>2127</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>2124</v>
+        <v>2125</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -25430,13 +25488,13 @@
         <v>210</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2127</v>
+        <v>2128</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>2128</v>
+        <v>2129</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -25450,13 +25508,13 @@
         <v>384</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2129</v>
+        <v>2130</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>2130</v>
+        <v>2131</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -25481,16 +25539,16 @@
         <v>427</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>2133</v>
+        <v>2134</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>2134</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25503,22 +25561,22 @@
       <c r="C9" s="1"/>
       <c r="D9" s="38"/>
       <c r="E9" s="1" t="s">
+        <v>2136</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>2136</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>2132</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>2133</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>2134</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>2135</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>2135</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>2131</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>2132</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>2133</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>2134</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25531,27 +25589,27 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>2136</v>
+        <v>2137</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>2136</v>
+        <v>2137</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>2133</v>
+        <v>2134</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>2134</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>2094</v>
+        <v>74</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>88</v>
@@ -25559,55 +25617,61 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>2094</v>
+        <v>2138</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>2133</v>
+        <v>2139</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>2134</v>
+        <v>2140</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>2141</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>74</v>
+      <c r="A12" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>2137</v>
+      <c r="E12" s="2" t="s">
+        <v>2142</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>2131</v>
+        <v>2143</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>2132</v>
+        <v>2144</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>2133</v>
+        <v>2145</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>2134</v>
+        <v>2146</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>2147</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>2138</v>
+      <c r="A13" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>88</v>
@@ -25615,55 +25679,61 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>2137</v>
+        <v>2148</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>2133</v>
+        <v>2149</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>2134</v>
+        <v>2150</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>2151</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>109</v>
+      <c r="A14" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="2" t="s">
-        <v>2139</v>
+      <c r="E14" s="1" t="s">
+        <v>2152</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>2140</v>
+        <v>2132</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>2141</v>
+        <v>2133</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>2133</v>
+        <v>2153</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>2134</v>
+        <v>2154</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>2155</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>89</v>
+        <v>440</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>88</v>
@@ -25671,55 +25741,61 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>2142</v>
+        <v>2156</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>2131</v>
+        <v>2143</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>2132</v>
+        <v>2144</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>2133</v>
+        <v>2157</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>2134</v>
+        <v>2158</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>2159</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>98</v>
+      <c r="A16" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>2143</v>
+      <c r="E16" s="2" t="s">
+        <v>2160</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>2144</v>
+        <v>2161</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>2145</v>
+        <v>2162</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>2163</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>440</v>
+        <v>401</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>88</v>
@@ -25727,27 +25803,30 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>2146</v>
+        <v>2164</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>2140</v>
+        <v>2132</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>2141</v>
+        <v>2133</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>2133</v>
+        <v>2165</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>2147</v>
+        <v>2166</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>2167</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>104</v>
+        <v>374</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>88</v>
@@ -25755,140 +25834,85 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="2" t="s">
-        <v>2148</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>2137</v>
+        <v>2168</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>2168</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>2144</v>
+        <v>2134</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>2145</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>401</v>
+      <c r="A19" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>2149</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>2137</v>
+      <c r="E19" s="2" t="s">
+        <v>2169</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>2169</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>2133</v>
+        <v>2134</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>2134</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>374</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>2150</v>
+        <v>2170</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>2150</v>
+        <v>2170</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>2133</v>
+        <v>2171</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>2134</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2" t="s">
-        <v>2151</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>2151</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>2131</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>2132</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>2133</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>2134</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
-        <v>2152</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>2152</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>2131</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>2132</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>2153</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>2134</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>2154</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>2135</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -25919,7 +25943,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>2155</v>
+        <v>2173</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>2</v>
@@ -27690,7 +27714,7 @@
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32209,10 +32233,10 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="Q54" activeCellId="0" sqref="Q54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>